<commit_message>
desafios adicionados e resolvidos
</commit_message>
<xml_diff>
--- a/modulo-02/d013/Desafio 013 - Base.xlsx
+++ b/modulo-02/d013/Desafio 013 - Base.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,50 @@
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -68,7 +112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -84,6 +128,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -388,7 +441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -522,13 +575,84 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:E4"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B5:E5"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>